<commit_message>
Updated process to select between two template versions
</commit_message>
<xml_diff>
--- a/create_agent_directory/resources/enhanced_template.xlsx
+++ b/create_agent_directory/resources/enhanced_template.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Data Entry" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Data Entry'!$A$1:$BK$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Data Entry'!$A$1:$AW$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -345,29 +345,21 @@
     </comment>
     <comment ref="L1" authorId="0" shapeId="0">
       <text>
-        <t>Number of files needed to answer query
-Number of files required for the ground truth response
-REQUIRED FIELD
-Format: Number</t>
-      </text>
-    </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
-      <text>
         <t>Can be answered from knowledge corpus?
 OPTIONS: Yes, No
 REQUIRED FIELD
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">Justification if cannot be answered from knowledge corpus
 </t>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
-      <text>
-        <t xml:space="preserve">Ground truth file reference1
+    <comment ref="N1" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">Ground truth file reference
 Name of the files required for the ground truth response
 Notes:
 * Do not enter SharePoint URLs to the files here! Only the base file names.
@@ -376,16 +368,16 @@
 </t>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
-      <text>
-        <t xml:space="preserve">Knowledge corpus file type2
+    <comment ref="O1" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">Knowledge corpus file type
 File type of the files required for the ground truth response. 
 Word documents (DOC/DOCX), PowerPoint (PPT/PPTX), PDF files, Excel (xls, xlsx), Text (.txt, .md, .log), HTML (html, htm), CSV (csv), SharePoint site containing Plain text (ASPX file), SharePoint - Word documents (DOC/DOCX), SharePoint - PowerPoint (PPT/PPTX), SharePoint - PDF files
 REQUIRED FIELD
 </t>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <t>File size type
 File size type for the files required for ground truth response
@@ -394,7 +386,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <t>File size for PDFs, Power Point, Word doc, Text, SharePoint library docs, Worksheets
 File size of the files required for the ground response.
@@ -410,7 +402,7 @@
 Format: Number</t>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <t>Textual body
 Is the ground truth snippet from a textual body within the file?
@@ -421,7 +413,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <t>Simple Header
 Is the ground truth snippet from a simple header within the file?
@@ -432,7 +424,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0">
+    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <t>Complex Header
 Is the ground truth snippet from a complex header within the file?
@@ -443,7 +435,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <t>Footnotes
 Is the ground truth snippet from a footnote within the file?
@@ -454,7 +446,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="W1" authorId="0" shapeId="0">
+    <comment ref="V1" authorId="0" shapeId="0">
       <text>
         <t>Simple Table
 Is the ground truth snippet from a simple table within the file?
@@ -465,7 +457,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0">
+    <comment ref="W1" authorId="0" shapeId="0">
       <text>
         <t>Complex Table
 Is the ground truth snippet from a complex table within the file?
@@ -476,7 +468,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0" shapeId="0">
+    <comment ref="X1" authorId="0" shapeId="0">
       <text>
         <t>PDF images
 Is the ground truth snippet from a pdf image within the file?
@@ -487,7 +479,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="Y1" authorId="0" shapeId="0">
       <text>
         <t>Charts
 Is the ground truth snippet from a chart within the file?
@@ -498,7 +490,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0" shapeId="0">
+    <comment ref="Z1" authorId="0" shapeId="0">
       <text>
         <t>Simple list
 Is the ground truth snippet from a simple list within the file?
@@ -509,7 +501,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0" shapeId="0">
+    <comment ref="AA1" authorId="0" shapeId="0">
       <text>
         <t>Complex list
 Is the ground truth snippet from a complex list within the file?
@@ -520,7 +512,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0" shapeId="0">
+    <comment ref="AB1" authorId="0" shapeId="0">
       <text>
         <t>Metadata
 Is the ground truth snippet from a metadata within the file?
@@ -531,7 +523,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0" shapeId="0">
+    <comment ref="AC1" authorId="0" shapeId="0">
       <text>
         <t>Content Page Number
 Indicate the locatio(s) where the ground truth snippet(s) can be found in the file.
@@ -548,7 +540,7 @@
 Format: Number</t>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0" shapeId="0">
+    <comment ref="AD1" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">User Query
 Enter the user query.
@@ -559,7 +551,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0" shapeId="0">
+    <comment ref="AE1" authorId="0" shapeId="0">
       <text>
         <t>Clarity of question
 What is the clarity of the question?
@@ -572,7 +564,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0" shapeId="0">
+    <comment ref="AF1" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">User question intent
 Allowed query types are:
@@ -581,7 +573,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0" shapeId="0">
+    <comment ref="AG1" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">Question length
 Short queries: Shorter than 5 tokens ("Short query")
@@ -595,7 +587,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0" shapeId="0">
+    <comment ref="AH1" authorId="0" shapeId="0">
       <text>
         <t>Keyword queries
 Queries that consist of only the important identifier word 
@@ -604,7 +596,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0" shapeId="0">
+    <comment ref="AI1" authorId="0" shapeId="0">
       <text>
         <t>Spelling errors
 Does the query contain spelling errors?
@@ -613,7 +605,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0" shapeId="0">
+    <comment ref="AJ1" authorId="0" shapeId="0">
       <text>
         <t>Doc term overlap
 Queries where the response uses different words and phrases from the question.
@@ -623,7 +615,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0" shapeId="0">
+    <comment ref="AK1" authorId="0" shapeId="0">
       <text>
         <t>Web search-engine-style queries
 Queries like those commonly entered into search engine
@@ -635,7 +627,7 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0" shapeId="0">
+    <comment ref="AL1" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">MCS agent responses
 Copy the full MCS agent response here, including the citation positions.
@@ -645,7 +637,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0" shapeId="0">
+    <comment ref="AM1" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">Expected response
 Ground truth
@@ -653,7 +645,19 @@
 </t>
       </text>
     </comment>
+    <comment ref="AN1" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">Expected tool selection
+</t>
+      </text>
+    </comment>
     <comment ref="AO1" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">Expeted tool parameters
+</t>
+      </text>
+    </comment>
+    <comment ref="AP1" authorId="0" shapeId="0">
       <text>
         <t>Ground truth snippets(Parsed) from files
 You need to include the actual text as well, not just the file name and page number. Pictures or screenshots are also acceptable in case of tables or images.
@@ -668,197 +672,7 @@
 Format: Number</t>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0" shapeId="0">
-      <text>
-        <t>Does the agent response answer the question?
-The options : 
-Yes - if the agent answers anything except “ I’m sorry,..”, otherwise No
-No - (declines to answer, empty response, error code) 
-OPTIONS: Yes, No
-REQUIRED FIELD
-Format: Dropdown</t>
-      </text>
-    </comment>
     <comment ref="AQ1" authorId="0" shapeId="0">
-      <text>
-        <t>Is the response comprehensive?
-This question assesses whether the response covers all key aspects of the ground truth.
-It is directly tied to the "Usefulness" dimension in the benchmarking rubric, specifically evaluating completeness.
-Fully complete:
-- Covers all parts of ground truth.
-- Critical points are covered in that response from SME perspective.
-- The response is complete and detailed.
-Somewhat complete:
-- The above criteria are only partly met.
-Not applicable:
-- No points from ground truth are covered.
-OPTIONS: Fully comprehensive, Somewhat comprehensive, Not applicable
-REQUIRED FIELD
-Format: Dropdown</t>
-      </text>
-    </comment>
-    <comment ref="AR1" authorId="0" shapeId="0">
-      <text>
-        <t>Is the response correct?
-Based on the ground truth, is the agent’s response, correct?
-Are the points in the response found in the ground truth?
-Does the response stays on topic?
-Is it directly tied to the “Correctness” and "Relevance" dimension in the benchmarking rubric?
-Comprehensiveness and correctness are complimentary.
-Correctness is a more nuanced aspect of comprehensiveness.
-Options are: 
-Fully correct (all points match what’s in the ground truth)
-Partially correct (only some point match the ground truth)
-Incorrect (no points match the ground truth)
-Example: Let’s say ground truth has points A and B, and the agent’s response has points A, B and C – this would be partially correct 
-Example 2: Let’s say ground truth has points A, B and C, and the agent’s response has points A, B – this would be fully correct 
-OPTIONS: Fully correct, Partially correct, Incorrect.
-REQUIRED FIELD
-Format: Dropdown</t>
-      </text>
-    </comment>
-    <comment ref="AS1" authorId="0" shapeId="0">
-      <text>
-        <t>Is the response's formatting good?
-This means the response is presented in a visually appealing way. 
-Options are: 
-Good, Acceptable or Bad.
-- Response has more effective highlighting.
-- Response clearly presents resources and examples.
-- Response uses bullet points or numbered list.
-- It is directly tied to the "Formatting" dimension in the benchmarking rubric.
-OPTIONS: Good, Acceptable, Bad
-REQUIRED FIELD
-Format: Number</t>
-      </text>
-    </comment>
-    <comment ref="AT1" authorId="0" shapeId="0">
-      <text>
-        <t>Does the response provide citation links?
-Options are: 
-- Yes
-- No
-Note: Bugs should be uncovered (let us know if you come across missing citations issues).
-OPTIONS: Yes, No
-REQUIRED FIELD
-Format: Dropdown</t>
-      </text>
-    </comment>
-    <comment ref="AU1" authorId="0" shapeId="0">
-      <text>
-        <t>If the response provides citations. Are the citations accurate/valid?
-This means that the response can be found in the cited documents even if the response is not correct.
-Options are: 
-- accurate
-- partially accurate
-- inaccurate
-The latter one includes hallucinations.
-OPTIONS: accurate, partially accurate, inaccurate
-REQUIRED FIELD
-Format: Dropdown</t>
-      </text>
-    </comment>
-    <comment ref="AV1" authorId="0" shapeId="0">
-      <text>
-        <t xml:space="preserve">Please provide all the links to the citations
-Enter the links from the files or locations used in the response.
-REQUIRED FIELD
-</t>
-      </text>
-    </comment>
-    <comment ref="AW1" authorId="0" shapeId="0">
-      <text>
-        <t>Overall what is the quality of the response?
-Overall, what is the quality of the response? If you were an end user, would you use this response?
-OPTIONS: Good, Acceptable, Bad
-REQUIRED FIELD
-Format: Dropdown</t>
-      </text>
-    </comment>
-    <comment ref="AX1" authorId="0" shapeId="0">
-      <text>
-        <t xml:space="preserve">What aspects of the response make it good quality (if applicable)?
-Please explain in what way the response is showing that it is of good quality
-</t>
-      </text>
-    </comment>
-    <comment ref="AY1" authorId="0" shapeId="0">
-      <text>
-        <t xml:space="preserve">What aspects of the response make it poor quality (if applicable)?
-Please explain in what way the response is deficient or lacking
-</t>
-      </text>
-    </comment>
-    <comment ref="AZ1" authorId="0" shapeId="0">
-      <text>
-        <t xml:space="preserve">Any additional comments or reasoning for the rating? Optional
-</t>
-      </text>
-    </comment>
-    <comment ref="BA1" authorId="0" shapeId="0">
-      <text>
-        <t>Did the agent follow the given instructions or context?
-OPTIONS: completely followed, partially followed, did not follow
-REQUIRED FIELD
-Format: Dropdown</t>
-      </text>
-    </comment>
-    <comment ref="BB1" authorId="0" shapeId="0">
-      <text>
-        <t>Logical flow, transitions, sentence structure.
-How is the given layout and structure helping to understand the response?
-Could it have been organized and flowed in a way that made more sense?
-Rate between 1 (very bad) and 5 (very good)
-OPTIONS: 1, 2, 3, 4, 5
-REQUIRED FIELD
-Format: Dropdown</t>
-      </text>
-    </comment>
-    <comment ref="BC1" authorId="0" shapeId="0">
-      <text>
-        <t>Does it sound fluent and natural to a native speaker?
-How is the quality of the grammar and natural use of English?
-Rate between 1 (very bad) and 5 (very good)
-OPTIONS: 1, 2, 3, 4, 5
-REQUIRED FIELD
-Format: Dropdown</t>
-      </text>
-    </comment>
-    <comment ref="BD1" authorId="0" shapeId="0">
-      <text>
-        <t>Check if content is biased, harmful, or toxic.
-OPTIONS: Yes, No
-REQUIRED FIELD
-Format: Dropdown</t>
-      </text>
-    </comment>
-    <comment ref="BE1" authorId="0" shapeId="0">
-      <text>
-        <t>What is the clarity of response?
- Is the response clear?
-Options are:
-Yes,No
-Yes: Response used simpler wording, explained terms or acronyms clearly and avoided technical jargon.
-No: Otherwise No
-It is directly tied to the "Clarity" dimension in the benchmarking rubric.
-OPTIONS: Yes, No
-REQUIRED FIELD
-Format: Dropdown</t>
-      </text>
-    </comment>
-    <comment ref="BF1" authorId="0" shapeId="0">
-      <text>
-        <t>What is the tone and writing style of the agent response?
-Options are:
-- Formal and conversational
-- Informal
-- Non-conversational
-OPTIONS: Formal and conversational, Informal, Non-conversational
-REQUIRED FIELD
-Format: Dropdown</t>
-      </text>
-    </comment>
-    <comment ref="BG1" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">Custom Rubric Used
 The custom rubric contains one or multiple rubric criteria (questions related to the current query - can be different for each query)
@@ -866,14 +680,14 @@
 </t>
       </text>
     </comment>
-    <comment ref="BH1" authorId="0" shapeId="0">
+    <comment ref="AR1" authorId="0" shapeId="0">
       <text>
         <t>Scores Per Rubric
 This is a range between -10 and +10
 Format: Number</t>
       </text>
     </comment>
-    <comment ref="BI1" authorId="0" shapeId="0">
+    <comment ref="AS1" authorId="0" shapeId="0">
       <text>
         <t>Final Rubric Score
 If the score given is greater than 0, the final rubric score if Yes
@@ -882,25 +696,33 @@
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="BJ1" authorId="0" shapeId="0">
+    <comment ref="AT1" authorId="0" shapeId="0">
       <text>
         <t>Pass/Fail
-Fail if: 
-Does the agent response answer the question? --&gt; partially answers, does not answer
-What is the quality of the response? --&gt; bad
-Is the response comprehensive? --&gt; Somewhat comprehensive, not comprehensive
-Is the response correct? --&gt; Partially correct, incorrect
-If the response provides citations. Are the citations accurate? --&gt; partially accurate, inaccurate
-Did the agent follow the instructions? ---&gt; partially followed, did not follow
 OPTIONS: Pass, Fail
 REQUIRED FIELD
 Format: Dropdown</t>
       </text>
     </comment>
-    <comment ref="BK1" authorId="0" shapeId="0">
+    <comment ref="AU1" authorId="0" shapeId="0">
       <text>
         <t xml:space="preserve">Justification for fail
 Give a short description why you selected Fail.
+REQUIRED FIELD
+</t>
+      </text>
+    </comment>
+    <comment ref="AV1" authorId="0" shapeId="0">
+      <text>
+        <t>Success score (1-5)
+OPTIONS: 1, 2, 3, 4, 5
+REQUIRED FIELD
+Format: Number</t>
+      </text>
+    </comment>
+    <comment ref="AW1" authorId="0" shapeId="0">
+      <text>
+        <t xml:space="preserve">Justification for Success score
 REQUIRED FIELD
 </t>
       </text>
@@ -1199,7 +1021,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -1669,20 +1491,20 @@
     <row r="15" ht="71" customHeight="1">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>Number of files needed to answer query</t>
-        </is>
-      </c>
-      <c r="B15" s="3" t="inlineStr">
-        <is>
-          <t>Number of files required for the ground truth response</t>
-        </is>
-      </c>
+          <t>Can be answered from knowledge corpus?</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr"/>
       <c r="C15" s="3" t="inlineStr">
         <is>
-          <t>Number</t>
-        </is>
-      </c>
-      <c r="D15" s="3" t="inlineStr"/>
+          <t>Dropdown</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>Yes, No</t>
+        </is>
+      </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
           <t>Single</t>
@@ -1695,27 +1517,23 @@
       </c>
       <c r="G15" s="3" t="inlineStr">
         <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" ht="71" customHeight="1">
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="89" customHeight="1">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>Can be answered from knowledge corpus?</t>
+          <t>Justification if cannot be answered from knowledge corpus</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr"/>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D16" s="3" t="inlineStr">
-        <is>
-          <t>Yes, No</t>
-        </is>
-      </c>
+          <t>Free text</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr"/>
       <c r="E16" s="3" t="inlineStr">
         <is>
           <t>Single</t>
@@ -1723,47 +1541,18 @@
       </c>
       <c r="F16" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G16" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" ht="89" customHeight="1">
+          <t>Optional</t>
+        </is>
+      </c>
+      <c r="G16" s="3" t="inlineStr"/>
+    </row>
+    <row r="17" ht="161" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Justification if cannot be answered from knowledge corpus</t>
-        </is>
-      </c>
-      <c r="B17" s="3" t="inlineStr"/>
-      <c r="C17" s="3" t="inlineStr">
-        <is>
-          <t>Free text</t>
-        </is>
-      </c>
-      <c r="D17" s="3" t="inlineStr"/>
-      <c r="E17" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F17" s="3" t="inlineStr">
-        <is>
-          <t>Optional</t>
-        </is>
-      </c>
-      <c r="G17" s="3" t="inlineStr"/>
-    </row>
-    <row r="18" ht="161" customHeight="1">
-      <c r="A18" s="3" t="inlineStr">
-        <is>
-          <t>Ground truth file reference1</t>
-        </is>
-      </c>
-      <c r="B18" s="3" t="inlineStr">
+          <t>Ground truth file reference</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
         <is>
           <t>Name of the files required for the ground truth response
 Notes:
@@ -1771,6 +1560,41 @@
 * Separate multiple files by an in-cell line break (double click in the field -&gt; ALT+ENTER)</t>
         </is>
       </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>Free text</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="inlineStr"/>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>Multiple</t>
+        </is>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>Directory_PolicyBasedScholarships_20HEIs_Vietnam_2024.docx
+Guidelines_StudyAbroad_ScholarshipApplicationProcess.html</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="215" customHeight="1">
+      <c r="A18" s="3" t="inlineStr">
+        <is>
+          <t>Knowledge corpus file type</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>File type of the files required for the ground truth response. 
+Word documents (DOC/DOCX), PowerPoint (PPT/PPTX), PDF files, Excel (xls, xlsx), Text (.txt, .md, .log), HTML (html, htm), CSV (csv), SharePoint site containing Plain text (ASPX file), SharePoint - Word documents (DOC/DOCX), SharePoint - PowerPoint (PPT/PPTX), SharePoint - PDF files</t>
+        </is>
+      </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
           <t>Free text</t>
@@ -1789,91 +1613,56 @@
       </c>
       <c r="G18" s="3" t="inlineStr">
         <is>
-          <t>Directory_PolicyBasedScholarships_20HEIs_Vietnam_2024.docx
-Guidelines_StudyAbroad_ScholarshipApplicationProcess.html</t>
-        </is>
-      </c>
-    </row>
-    <row r="19" ht="215" customHeight="1">
-      <c r="A19" s="3" t="inlineStr">
-        <is>
-          <t>Knowledge corpus file type2</t>
-        </is>
-      </c>
-      <c r="B19" s="3" t="inlineStr">
-        <is>
-          <t>File type of the files required for the ground truth response. 
-Word documents (DOC/DOCX), PowerPoint (PPT/PPTX), PDF files, Excel (xls, xlsx), Text (.txt, .md, .log), HTML (html, htm), CSV (csv), SharePoint site containing Plain text (ASPX file), SharePoint - Word documents (DOC/DOCX), SharePoint - PowerPoint (PPT/PPTX), SharePoint - PDF files</t>
-        </is>
-      </c>
-      <c r="C19" s="3" t="inlineStr">
-        <is>
-          <t>Free text</t>
-        </is>
-      </c>
-      <c r="D19" s="3" t="inlineStr"/>
-      <c r="E19" s="3" t="inlineStr">
-        <is>
-          <t>Multiple</t>
-        </is>
-      </c>
-      <c r="F19" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G19" s="3" t="inlineStr">
-        <is>
           <t>.docx
 .html</t>
         </is>
       </c>
     </row>
-    <row r="20" ht="71" customHeight="1">
-      <c r="A20" s="3" t="inlineStr">
+    <row r="19" ht="71" customHeight="1">
+      <c r="A19" s="3" t="inlineStr">
         <is>
           <t>File size type</t>
         </is>
       </c>
-      <c r="B20" s="3" t="inlineStr">
+      <c r="B19" s="3" t="inlineStr">
         <is>
           <t>File size type for the files required for ground truth response</t>
         </is>
       </c>
-      <c r="C20" s="3" t="inlineStr">
+      <c r="C19" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D20" s="3" t="inlineStr">
+      <c r="D19" s="3" t="inlineStr">
         <is>
           <t>Small, Medium, Large</t>
         </is>
       </c>
-      <c r="E20" s="3" t="inlineStr">
+      <c r="E19" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F20" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G20" s="3" t="inlineStr">
+      <c r="F19" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G19" s="3" t="inlineStr">
         <is>
           <t>Medium
 Small</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="233" customHeight="1">
-      <c r="A21" s="3" t="inlineStr">
+    <row r="20" ht="233" customHeight="1">
+      <c r="A20" s="3" t="inlineStr">
         <is>
           <t>File size for PDFs, Power Point, Word doc, Text, SharePoint library docs, Worksheets</t>
         </is>
       </c>
-      <c r="B21" s="3" t="inlineStr">
+      <c r="B20" s="3" t="inlineStr">
         <is>
           <t>File size of the files required for the ground response.
 The file size depending on the file type:
@@ -1886,476 +1675,476 @@
 So e.g. just enter 23 for a document with 23 pages.</t>
         </is>
       </c>
-      <c r="C21" s="3" t="inlineStr">
+      <c r="C20" s="3" t="inlineStr">
         <is>
           <t>Number</t>
         </is>
       </c>
-      <c r="D21" s="3" t="inlineStr"/>
-      <c r="E21" s="3" t="inlineStr">
+      <c r="D20" s="3" t="inlineStr"/>
+      <c r="E20" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F21" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G21" s="3" t="inlineStr">
+      <c r="F20" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G20" s="3" t="inlineStr">
         <is>
           <t>24
 1</t>
         </is>
       </c>
     </row>
-    <row r="22" ht="143" customHeight="1">
-      <c r="A22" s="3" t="inlineStr">
+    <row r="21" ht="143" customHeight="1">
+      <c r="A21" s="3" t="inlineStr">
         <is>
           <t>Textual body</t>
         </is>
       </c>
-      <c r="B22" s="3" t="inlineStr">
+      <c r="B21" s="3" t="inlineStr">
         <is>
           <t>Is the ground truth snippet from a textual body within the file?
 * Only enter Yes or No values
 * Separate responses per file by an in-cell line break (double click in the field -&gt; ALT+ENTER)</t>
         </is>
       </c>
-      <c r="C22" s="3" t="inlineStr">
+      <c r="C21" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D22" s="3" t="inlineStr">
+      <c r="D21" s="3" t="inlineStr">
         <is>
           <t>Yes, No</t>
         </is>
       </c>
-      <c r="E22" s="3" t="inlineStr">
+      <c r="E21" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F22" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G22" s="3" t="inlineStr">
+      <c r="F21" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G21" s="3" t="inlineStr">
         <is>
           <t>Yes
 Yes</t>
         </is>
       </c>
     </row>
-    <row r="23" ht="143" customHeight="1">
-      <c r="A23" s="3" t="inlineStr">
+    <row r="22" ht="143" customHeight="1">
+      <c r="A22" s="3" t="inlineStr">
         <is>
           <t>Simple Header</t>
         </is>
       </c>
-      <c r="B23" s="3" t="inlineStr">
+      <c r="B22" s="3" t="inlineStr">
         <is>
           <t>Is the ground truth snippet from a simple header within the file?
 * Only enter Yes or No values
 * Separate responses per file by an in-cell line break (double click in the field -&gt; ALT+ENTER)</t>
         </is>
       </c>
-      <c r="C23" s="3" t="inlineStr">
+      <c r="C22" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D23" s="3" t="inlineStr">
+      <c r="D22" s="3" t="inlineStr">
         <is>
           <t>Yes, No</t>
         </is>
       </c>
-      <c r="E23" s="3" t="inlineStr">
+      <c r="E22" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F23" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G23" s="3" t="inlineStr">
+      <c r="F22" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G22" s="3" t="inlineStr">
         <is>
           <t>No
 Yes</t>
         </is>
       </c>
     </row>
-    <row r="24" ht="143" customHeight="1">
-      <c r="A24" s="3" t="inlineStr">
+    <row r="23" ht="143" customHeight="1">
+      <c r="A23" s="3" t="inlineStr">
         <is>
           <t>Complex Header</t>
         </is>
       </c>
-      <c r="B24" s="3" t="inlineStr">
+      <c r="B23" s="3" t="inlineStr">
         <is>
           <t>Is the ground truth snippet from a complex header within the file?
 * Only enter Yes or No values
 * Separate responses per file by an in-cell line break (double click in the field -&gt; ALT+ENTER)</t>
         </is>
       </c>
-      <c r="C24" s="3" t="inlineStr">
+      <c r="C23" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D24" s="3" t="inlineStr">
+      <c r="D23" s="3" t="inlineStr">
         <is>
           <t>Yes, No</t>
         </is>
       </c>
-      <c r="E24" s="3" t="inlineStr">
+      <c r="E23" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F24" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G24" s="3" t="inlineStr">
+      <c r="F23" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G23" s="3" t="inlineStr">
         <is>
           <t>Yes
 No</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="143" customHeight="1">
-      <c r="A25" s="3" t="inlineStr">
+    <row r="24" ht="143" customHeight="1">
+      <c r="A24" s="3" t="inlineStr">
         <is>
           <t>Footnotes</t>
         </is>
       </c>
-      <c r="B25" s="3" t="inlineStr">
+      <c r="B24" s="3" t="inlineStr">
         <is>
           <t>Is the ground truth snippet from a footnote within the file?
 * Only enter Yes or No values
 * Separate responses per file by an in-cell line break (double click in the field -&gt; ALT+ENTER)</t>
         </is>
       </c>
-      <c r="C25" s="3" t="inlineStr">
+      <c r="C24" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D25" s="3" t="inlineStr">
+      <c r="D24" s="3" t="inlineStr">
         <is>
           <t>Yes, No</t>
         </is>
       </c>
-      <c r="E25" s="3" t="inlineStr">
+      <c r="E24" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F25" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G25" s="3" t="inlineStr">
+      <c r="F24" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G24" s="3" t="inlineStr">
         <is>
           <t>No
 No</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="143" customHeight="1">
-      <c r="A26" s="3" t="inlineStr">
+    <row r="25" ht="143" customHeight="1">
+      <c r="A25" s="3" t="inlineStr">
         <is>
           <t>Simple Table</t>
         </is>
       </c>
-      <c r="B26" s="3" t="inlineStr">
+      <c r="B25" s="3" t="inlineStr">
         <is>
           <t>Is the ground truth snippet from a simple table within the file?
 * Only enter Yes or No values
 * Separate responses per file by an in-cell line break (double click in the field -&gt; ALT+ENTER)</t>
         </is>
       </c>
-      <c r="C26" s="3" t="inlineStr">
+      <c r="C25" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D26" s="3" t="inlineStr">
+      <c r="D25" s="3" t="inlineStr">
         <is>
           <t>Yes, No</t>
         </is>
       </c>
-      <c r="E26" s="3" t="inlineStr">
+      <c r="E25" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F26" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G26" s="3" t="inlineStr">
+      <c r="F25" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G25" s="3" t="inlineStr">
         <is>
           <t>Yes
 No</t>
         </is>
       </c>
     </row>
-    <row r="27" ht="143" customHeight="1">
-      <c r="A27" s="3" t="inlineStr">
+    <row r="26" ht="143" customHeight="1">
+      <c r="A26" s="3" t="inlineStr">
         <is>
           <t>Complex Table</t>
         </is>
       </c>
-      <c r="B27" s="3" t="inlineStr">
+      <c r="B26" s="3" t="inlineStr">
         <is>
           <t>Is the ground truth snippet from a complex table within the file?
 * Only enter Yes or No values
 * Separate responses per file by an in-cell line break (double click in the field -&gt; ALT+ENTER)</t>
         </is>
       </c>
-      <c r="C27" s="3" t="inlineStr">
+      <c r="C26" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D27" s="3" t="inlineStr">
+      <c r="D26" s="3" t="inlineStr">
         <is>
           <t>Yes, No</t>
         </is>
       </c>
-      <c r="E27" s="3" t="inlineStr">
+      <c r="E26" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F27" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G27" s="3" t="inlineStr">
+      <c r="F26" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G26" s="3" t="inlineStr">
         <is>
           <t>No
 No</t>
         </is>
       </c>
     </row>
-    <row r="28" ht="143" customHeight="1">
-      <c r="A28" s="3" t="inlineStr">
+    <row r="27" ht="143" customHeight="1">
+      <c r="A27" s="3" t="inlineStr">
         <is>
           <t>PDF images</t>
         </is>
       </c>
-      <c r="B28" s="3" t="inlineStr">
+      <c r="B27" s="3" t="inlineStr">
         <is>
           <t>Is the ground truth snippet from a pdf image within the file?
 * Only enter Yes or No values
 * Separate responses per file by an in-cell line break (double click in the field -&gt; ALT+ENTER)</t>
         </is>
       </c>
-      <c r="C28" s="3" t="inlineStr">
+      <c r="C27" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D28" s="3" t="inlineStr">
+      <c r="D27" s="3" t="inlineStr">
         <is>
           <t>Yes, No</t>
         </is>
       </c>
-      <c r="E28" s="3" t="inlineStr">
+      <c r="E27" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F28" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G28" s="3" t="inlineStr">
+      <c r="F27" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G27" s="3" t="inlineStr">
         <is>
           <t>No
 No</t>
         </is>
       </c>
     </row>
-    <row r="29" ht="143" customHeight="1">
-      <c r="A29" s="3" t="inlineStr">
+    <row r="28" ht="143" customHeight="1">
+      <c r="A28" s="3" t="inlineStr">
         <is>
           <t>Charts</t>
         </is>
       </c>
-      <c r="B29" s="3" t="inlineStr">
+      <c r="B28" s="3" t="inlineStr">
         <is>
           <t>Is the ground truth snippet from a chart within the file?
 * Only enter Yes or No values
 * Separate responses per file by an in-cell line break (double click in the field -&gt; ALT+ENTER)</t>
         </is>
       </c>
-      <c r="C29" s="3" t="inlineStr">
+      <c r="C28" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D29" s="3" t="inlineStr">
+      <c r="D28" s="3" t="inlineStr">
         <is>
           <t>Yes, No</t>
         </is>
       </c>
-      <c r="E29" s="3" t="inlineStr">
+      <c r="E28" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F29" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G29" s="3" t="inlineStr">
+      <c r="F28" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G28" s="3" t="inlineStr">
         <is>
           <t>No
 No</t>
         </is>
       </c>
     </row>
-    <row r="30" ht="143" customHeight="1">
-      <c r="A30" s="3" t="inlineStr">
+    <row r="29" ht="143" customHeight="1">
+      <c r="A29" s="3" t="inlineStr">
         <is>
           <t>Simple list</t>
         </is>
       </c>
-      <c r="B30" s="3" t="inlineStr">
+      <c r="B29" s="3" t="inlineStr">
         <is>
           <t>Is the ground truth snippet from a simple list within the file?
 * Only enter Yes or No values
 * Separate responses per file by an in-cell line break (double click in the field -&gt; ALT+ENTER)</t>
         </is>
       </c>
-      <c r="C30" s="3" t="inlineStr">
+      <c r="C29" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D30" s="3" t="inlineStr">
+      <c r="D29" s="3" t="inlineStr">
         <is>
           <t>Yes, No</t>
         </is>
       </c>
-      <c r="E30" s="3" t="inlineStr">
+      <c r="E29" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F30" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G30" s="3" t="inlineStr">
+      <c r="F29" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G29" s="3" t="inlineStr">
         <is>
           <t>Yes
 Yes</t>
         </is>
       </c>
     </row>
-    <row r="31" ht="143" customHeight="1">
-      <c r="A31" s="3" t="inlineStr">
+    <row r="30" ht="143" customHeight="1">
+      <c r="A30" s="3" t="inlineStr">
         <is>
           <t>Complex list</t>
         </is>
       </c>
-      <c r="B31" s="3" t="inlineStr">
+      <c r="B30" s="3" t="inlineStr">
         <is>
           <t>Is the ground truth snippet from a complex list within the file?
 * Only enter Yes or No values
 * Separate responses per file by an in-cell line break (double click in the field -&gt; ALT+ENTER)</t>
         </is>
       </c>
-      <c r="C31" s="3" t="inlineStr">
+      <c r="C30" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D31" s="3" t="inlineStr">
+      <c r="D30" s="3" t="inlineStr">
         <is>
           <t>Yes, No</t>
         </is>
       </c>
-      <c r="E31" s="3" t="inlineStr">
+      <c r="E30" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F31" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G31" s="3" t="inlineStr">
+      <c r="F30" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G30" s="3" t="inlineStr">
         <is>
           <t>No
 No</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="143" customHeight="1">
-      <c r="A32" s="3" t="inlineStr">
+    <row r="31" ht="143" customHeight="1">
+      <c r="A31" s="3" t="inlineStr">
         <is>
           <t>Metadata</t>
         </is>
       </c>
-      <c r="B32" s="3" t="inlineStr">
+      <c r="B31" s="3" t="inlineStr">
         <is>
           <t>Is the ground truth snippet from a metadata within the file?
 * Only enter Yes or No values
 * Separate responses per file by an in-cell line break (double click in the field -&gt; ALT+ENTER)</t>
         </is>
       </c>
-      <c r="C32" s="3" t="inlineStr">
+      <c r="C31" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D32" s="3" t="inlineStr">
+      <c r="D31" s="3" t="inlineStr">
         <is>
           <t>Yes, No</t>
         </is>
       </c>
-      <c r="E32" s="3" t="inlineStr">
+      <c r="E31" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F32" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G32" s="3" t="inlineStr">
+      <c r="F31" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G31" s="3" t="inlineStr">
         <is>
           <t>Yes
 Yes</t>
         </is>
       </c>
     </row>
-    <row r="33" ht="323" customHeight="1">
-      <c r="A33" s="3" t="inlineStr">
+    <row r="32" ht="323" customHeight="1">
+      <c r="A32" s="3" t="inlineStr">
         <is>
           <t>Content Page Number</t>
         </is>
       </c>
-      <c r="B33" s="3" t="inlineStr">
+      <c r="B32" s="3" t="inlineStr">
         <is>
           <t>Indicate the locatio(s) where the ground truth snippet(s) can be found in the file.
 Depending on the file type the location indicator can be:
@@ -2369,23 +2158,23 @@
 The example shows three files with several occurrence locations.</t>
         </is>
       </c>
-      <c r="C33" s="3" t="inlineStr">
+      <c r="C32" s="3" t="inlineStr">
         <is>
           <t>Number</t>
         </is>
       </c>
-      <c r="D33" s="3" t="inlineStr"/>
-      <c r="E33" s="3" t="inlineStr">
+      <c r="D32" s="3" t="inlineStr"/>
+      <c r="E32" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F33" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G33" s="3" t="inlineStr">
+      <c r="F32" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G32" s="3" t="inlineStr">
         <is>
           <t>3,6,22
 5
@@ -2393,13 +2182,13 @@
         </is>
       </c>
     </row>
-    <row r="34" ht="107" customHeight="1">
-      <c r="A34" s="3" t="inlineStr">
+    <row r="33" ht="107" customHeight="1">
+      <c r="A33" s="3" t="inlineStr">
         <is>
           <t>User Query</t>
         </is>
       </c>
-      <c r="B34" s="3" t="inlineStr">
+      <c r="B33" s="3" t="inlineStr">
         <is>
           <t>Enter the user query.
 IMPORTANT: 
@@ -2407,35 +2196,35 @@
 * Do NOT enter more than one turn per row!</t>
         </is>
       </c>
-      <c r="C34" s="3" t="inlineStr">
+      <c r="C33" s="3" t="inlineStr">
         <is>
           <t>Free text</t>
         </is>
       </c>
-      <c r="D34" s="3" t="inlineStr"/>
-      <c r="E34" s="3" t="inlineStr">
+      <c r="D33" s="3" t="inlineStr"/>
+      <c r="E33" s="3" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="F34" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G34" s="3" t="inlineStr">
+      <c r="F33" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G33" s="3" t="inlineStr">
         <is>
           <t>I want to find a full scholarship to study Engineering in Australia.  what the minimum IELTS requirement is?</t>
         </is>
       </c>
     </row>
-    <row r="35" ht="143" customHeight="1">
-      <c r="A35" s="3" t="inlineStr">
+    <row r="34" ht="143" customHeight="1">
+      <c r="A34" s="3" t="inlineStr">
         <is>
           <t>Clarity of question</t>
         </is>
       </c>
-      <c r="B35" s="3" t="inlineStr">
+      <c r="B34" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">What is the clarity of the question?
 User personas should ask questions varying in clarity: 
@@ -2444,75 +2233,75 @@
 * High (Perfectly Complete) </t>
         </is>
       </c>
-      <c r="C35" s="3" t="inlineStr">
+      <c r="C34" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D35" s="3" t="inlineStr">
+      <c r="D34" s="3" t="inlineStr">
         <is>
           <t>Low,  
 Medium,  
 High</t>
         </is>
       </c>
-      <c r="E35" s="3" t="inlineStr">
+      <c r="E34" s="3" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="F35" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G35" s="3" t="inlineStr">
+      <c r="F34" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G34" s="3" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="161" customHeight="1">
-      <c r="A36" s="3" t="inlineStr">
+    <row r="35" ht="161" customHeight="1">
+      <c r="A35" s="3" t="inlineStr">
         <is>
           <t>User question intent</t>
         </is>
       </c>
-      <c r="B36" s="3" t="inlineStr">
+      <c r="B35" s="3" t="inlineStr">
         <is>
           <t>Allowed query types are:
 "fact_seeking, procedural, summarization, comparison, general_multi_part, clarifying, reason_seeking, status_related, resource_seeking, feedback_and_assistance, hypothetical, two_turn_conversation"</t>
         </is>
       </c>
-      <c r="C36" s="3" t="inlineStr">
+      <c r="C35" s="3" t="inlineStr">
         <is>
           <t>Free text</t>
         </is>
       </c>
-      <c r="D36" s="3" t="inlineStr"/>
-      <c r="E36" s="3" t="inlineStr">
+      <c r="D35" s="3" t="inlineStr"/>
+      <c r="E35" s="3" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="F36" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G36" s="3" t="inlineStr">
+      <c r="F35" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G35" s="3" t="inlineStr">
         <is>
           <t>fact_seeking</t>
         </is>
       </c>
     </row>
-    <row r="37" ht="215" customHeight="1">
-      <c r="A37" s="3" t="inlineStr">
+    <row r="36" ht="215" customHeight="1">
+      <c r="A36" s="3" t="inlineStr">
         <is>
           <t>Question length</t>
         </is>
       </c>
-      <c r="B37" s="3" t="inlineStr">
+      <c r="B36" s="3" t="inlineStr">
         <is>
           <t>Short queries: Shorter than 5 tokens ("Short query")
 Medium queries: Between 5 and 20 tokens ("This is a medium query length")
@@ -2523,12 +2312,49 @@
 * Long (# tokens)</t>
         </is>
       </c>
+      <c r="C36" s="3" t="inlineStr">
+        <is>
+          <t>Free text</t>
+        </is>
+      </c>
+      <c r="D36" s="3" t="inlineStr"/>
+      <c r="E36" s="3" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="F36" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G36" s="3" t="inlineStr">
+        <is>
+          <t>Long (22 tokens)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37" ht="71" customHeight="1">
+      <c r="A37" s="3" t="inlineStr">
+        <is>
+          <t>Keyword queries</t>
+        </is>
+      </c>
+      <c r="B37" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Queries that consist of only the important identifier word </t>
+        </is>
+      </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>Free text</t>
-        </is>
-      </c>
-      <c r="D37" s="3" t="inlineStr"/>
+          <t>Dropdown</t>
+        </is>
+      </c>
+      <c r="D37" s="3" t="inlineStr">
+        <is>
+          <t>Yes, No</t>
+        </is>
+      </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
           <t>Single</t>
@@ -2541,19 +2367,19 @@
       </c>
       <c r="G37" s="3" t="inlineStr">
         <is>
-          <t>Long (22 tokens)</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
     <row r="38" ht="71" customHeight="1">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>Keyword queries</t>
+          <t>Spelling errors</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Queries that consist of only the important identifier word </t>
+          <t>Does the query contain spelling errors?</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
@@ -2578,92 +2404,55 @@
       </c>
       <c r="G38" s="3" t="inlineStr">
         <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="39" ht="71" customHeight="1">
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="39" ht="107" customHeight="1">
       <c r="A39" s="3" t="inlineStr">
         <is>
-          <t>Spelling errors</t>
+          <t>Doc term overlap</t>
         </is>
       </c>
       <c r="B39" s="3" t="inlineStr">
-        <is>
-          <t>Does the query contain spelling errors?</t>
-        </is>
-      </c>
-      <c r="C39" s="3" t="inlineStr">
-        <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D39" s="3" t="inlineStr">
-        <is>
-          <t>Yes, No</t>
-        </is>
-      </c>
-      <c r="E39" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F39" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G39" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="40" ht="107" customHeight="1">
-      <c r="A40" s="3" t="inlineStr">
-        <is>
-          <t>Doc term overlap</t>
-        </is>
-      </c>
-      <c r="B40" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">Queries where the response uses different words and phrases from the question.
 This can be challenging for a retrieval engine to find. </t>
         </is>
       </c>
-      <c r="C40" s="3" t="inlineStr">
+      <c r="C39" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D40" s="3" t="inlineStr">
+      <c r="D39" s="3" t="inlineStr">
         <is>
           <t>Yes, No</t>
         </is>
       </c>
-      <c r="E40" s="3" t="inlineStr">
+      <c r="E39" s="3" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="F40" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G40" s="3" t="inlineStr">
+      <c r="F39" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G39" s="3" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
     </row>
-    <row r="41" ht="233" customHeight="1">
-      <c r="A41" s="3" t="inlineStr">
+    <row r="40" ht="233" customHeight="1">
+      <c r="A40" s="3" t="inlineStr">
         <is>
           <t>Web search-engine-style queries</t>
         </is>
       </c>
-      <c r="B41" s="3" t="inlineStr">
+      <c r="B40" s="3" t="inlineStr">
         <is>
           <t>Queries like those commonly entered into search engine
 For example "best retrieval concept queries":
@@ -2671,62 +2460,62 @@
 Example 2: "Summarize the main steps involved in the incident response process according to the NIST SP 800-61 guidelines."</t>
         </is>
       </c>
-      <c r="C41" s="3" t="inlineStr">
+      <c r="C40" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D41" s="3" t="inlineStr">
+      <c r="D40" s="3" t="inlineStr">
         <is>
           <t>Yes, No</t>
         </is>
       </c>
-      <c r="E41" s="3" t="inlineStr">
+      <c r="E40" s="3" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="F41" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G41" s="3" t="inlineStr">
+      <c r="F40" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G40" s="3" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
     </row>
-    <row r="42" ht="755" customHeight="1">
-      <c r="A42" s="3" t="inlineStr">
+    <row r="41" ht="755" customHeight="1">
+      <c r="A41" s="3" t="inlineStr">
         <is>
           <t>MCS agent responses</t>
         </is>
       </c>
-      <c r="B42" s="3" t="inlineStr">
+      <c r="B41" s="3" t="inlineStr">
         <is>
           <t>Copy the full MCS agent response here, including the citation positions.
 E.g. 
 Saturn is a planet [1][2]</t>
         </is>
       </c>
-      <c r="C42" s="3" t="inlineStr">
+      <c r="C41" s="3" t="inlineStr">
         <is>
           <t>Free text</t>
         </is>
       </c>
-      <c r="D42" s="3" t="inlineStr"/>
-      <c r="E42" s="3" t="inlineStr">
+      <c r="D41" s="3" t="inlineStr"/>
+      <c r="E41" s="3" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="F42" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G42" s="3" t="inlineStr">
+      <c r="F41" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G41" s="3" t="inlineStr">
         <is>
           <t>Here’s a summary of scholarship opportunities, eligibility, and application processes:
 Types of Scholarships:
@@ -2772,34 +2561,34 @@
         </is>
       </c>
     </row>
-    <row r="43" ht="305" customHeight="1">
-      <c r="A43" s="3" t="inlineStr">
+    <row r="42" ht="305" customHeight="1">
+      <c r="A42" s="3" t="inlineStr">
         <is>
           <t>Expected response</t>
         </is>
       </c>
-      <c r="B43" s="3" t="inlineStr">
+      <c r="B42" s="3" t="inlineStr">
         <is>
           <t>Ground truth</t>
         </is>
       </c>
-      <c r="C43" s="3" t="inlineStr">
+      <c r="C42" s="3" t="inlineStr">
         <is>
           <t>Free text</t>
         </is>
       </c>
-      <c r="D43" s="3" t="inlineStr"/>
-      <c r="E43" s="3" t="inlineStr">
+      <c r="D42" s="3" t="inlineStr"/>
+      <c r="E42" s="3" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="F43" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G43" s="3" t="inlineStr">
+      <c r="F42" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G42" s="3" t="inlineStr">
         <is>
           <t>There are several government-funded scholarships you can apply for to study Engineering in Australia as an international student.
 The most prestigious option is the Australia Awards Scholarship, funded by the Australian government. If you're from a partner country like Vietnam, you may qualify. This scholarship typically covers tuition, living expenses, return flights, and health insurance, making it a full-ride opportunity. It’s highly competitive, so strong academic and language qualifications are required.
@@ -2810,13 +2599,55 @@
         </is>
       </c>
     </row>
-    <row r="44" ht="251" customHeight="1">
+    <row r="43" ht="71" customHeight="1">
+      <c r="A43" s="3" t="inlineStr">
+        <is>
+          <t>Expected tool selection</t>
+        </is>
+      </c>
+      <c r="B43" s="3" t="inlineStr"/>
+      <c r="C43" s="3" t="inlineStr">
+        <is>
+          <t>Free text</t>
+        </is>
+      </c>
+      <c r="D43" s="3" t="inlineStr"/>
+      <c r="E43" s="3" t="inlineStr"/>
+      <c r="F43" s="3" t="inlineStr">
+        <is>
+          <t>Optional</t>
+        </is>
+      </c>
+      <c r="G43" s="3" t="inlineStr"/>
+    </row>
+    <row r="44" ht="71" customHeight="1">
       <c r="A44" s="3" t="inlineStr">
         <is>
+          <t>Expeted tool parameters</t>
+        </is>
+      </c>
+      <c r="B44" s="3" t="inlineStr"/>
+      <c r="C44" s="3" t="inlineStr">
+        <is>
+          <t>Free text</t>
+        </is>
+      </c>
+      <c r="D44" s="3" t="inlineStr"/>
+      <c r="E44" s="3" t="inlineStr"/>
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>Optional</t>
+        </is>
+      </c>
+      <c r="G44" s="3" t="inlineStr"/>
+    </row>
+    <row r="45" ht="251" customHeight="1">
+      <c r="A45" s="3" t="inlineStr">
+        <is>
           <t>Ground truth snippets(Parsed) from files</t>
         </is>
       </c>
-      <c r="B44" s="3" t="inlineStr">
+      <c r="B45" s="3" t="inlineStr">
         <is>
           <t>You need to include the actual text as well, not just the file name and page number. Pictures or screenshots are also acceptable in case of tables or images.
 It is important to follow this schema:
@@ -2828,23 +2659,23 @@
 etc.</t>
         </is>
       </c>
-      <c r="C44" s="3" t="inlineStr">
+      <c r="C45" s="3" t="inlineStr">
         <is>
           <t>Number</t>
         </is>
       </c>
-      <c r="D44" s="3" t="inlineStr"/>
-      <c r="E44" s="3" t="inlineStr">
+      <c r="D45" s="3" t="inlineStr"/>
+      <c r="E45" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F44" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G44" s="3" t="inlineStr">
+      <c r="F45" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G45" s="3" t="inlineStr">
         <is>
           <t>From: Guidelines_StudyAbroad_ScholarshipApplicationProcess.html
 3. Scholarship Type: Know What You're Applying For
@@ -2856,671 +2687,31 @@
         </is>
       </c>
     </row>
-    <row r="45" ht="125" customHeight="1">
-      <c r="A45" s="3" t="inlineStr">
-        <is>
-          <t>Does the agent response answer the question?</t>
-        </is>
-      </c>
-      <c r="B45" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">The options : 
-Yes - if the agent answers anything except “ I’m sorry,..”, otherwise No
-No - (declines to answer, empty response, error code) </t>
-        </is>
-      </c>
-      <c r="C45" s="3" t="inlineStr">
-        <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D45" s="3" t="inlineStr">
-        <is>
-          <t>Yes, No</t>
-        </is>
-      </c>
-      <c r="E45" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F45" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G45" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="46" ht="287" customHeight="1">
+    <row r="46" ht="161" customHeight="1">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>Is the response comprehensive?</t>
+          <t>Custom Rubric Used</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
-        <is>
-          <t>This question assesses whether the response covers all key aspects of the ground truth.
-It is directly tied to the "Usefulness" dimension in the benchmarking rubric, specifically evaluating completeness.
-Fully complete:
-- Covers all parts of ground truth.
-- Critical points are covered in that response from SME perspective.
-- The response is complete and detailed.
-Somewhat complete:
-- The above criteria are only partly met.
-Not applicable:
-- No points from ground truth are covered.</t>
-        </is>
-      </c>
-      <c r="C46" s="3" t="inlineStr">
-        <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D46" s="3" t="inlineStr">
-        <is>
-          <t>Fully comprehensive,Somewhat comprehensive,Not applicable</t>
-        </is>
-      </c>
-      <c r="E46" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F46" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G46" s="3" t="inlineStr">
-        <is>
-          <t>Somewhat comprehensive</t>
-        </is>
-      </c>
-    </row>
-    <row r="47" ht="449" customHeight="1">
-      <c r="A47" s="3" t="inlineStr">
-        <is>
-          <t>Is the response correct?</t>
-        </is>
-      </c>
-      <c r="B47" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Based on the ground truth, is the agent’s response, correct?
-Are the points in the response found in the ground truth?
-Does the response stays on topic?
-Is it directly tied to the “Correctness” and "Relevance" dimension in the benchmarking rubric?
-Comprehensiveness and correctness are complimentary.
-Correctness is a more nuanced aspect of comprehensiveness.
-Options are: 
-Fully correct (all points match what’s in the ground truth)
-Partially correct (only some point match the ground truth)
-Incorrect (no points match the ground truth)
-Example: Let’s say ground truth has points A and B, and the agent’s response has points A, B and C – this would be partially correct 
-Example 2: Let’s say ground truth has points A, B and C, and the agent’s response has points A, B – this would be fully correct </t>
-        </is>
-      </c>
-      <c r="C47" s="3" t="inlineStr">
-        <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D47" s="3" t="inlineStr">
-        <is>
-          <t>Fully correct, Partially correct, Incorrect.</t>
-        </is>
-      </c>
-      <c r="E47" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F47" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G47" s="3" t="inlineStr">
-        <is>
-          <t>partially correct</t>
-        </is>
-      </c>
-    </row>
-    <row r="48" ht="215" customHeight="1">
-      <c r="A48" s="3" t="inlineStr">
-        <is>
-          <t>Is the response's formatting good?</t>
-        </is>
-      </c>
-      <c r="B48" s="3" t="inlineStr">
-        <is>
-          <t>This means the response is presented in a visually appealing way. 
-Options are: 
-Good, Acceptable or Bad.
-- Response has more effective highlighting.
-- Response clearly presents resources and examples.
-- Response uses bullet points or numbered list.
-- It is directly tied to the "Formatting" dimension in the benchmarking rubric.</t>
-        </is>
-      </c>
-      <c r="C48" s="3" t="inlineStr">
-        <is>
-          <t>Number</t>
-        </is>
-      </c>
-      <c r="D48" s="3" t="inlineStr">
-        <is>
-          <t>Good, Acceptable, Bad</t>
-        </is>
-      </c>
-      <c r="E48" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F48" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G48" s="3" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-    </row>
-    <row r="49" ht="107" customHeight="1">
-      <c r="A49" s="3" t="inlineStr">
-        <is>
-          <t>Does the response provide citation links?</t>
-        </is>
-      </c>
-      <c r="B49" s="3" t="inlineStr">
-        <is>
-          <t>Options are: 
-- Yes
-- No
-Note: Bugs should be uncovered (let us know if you come across missing citations issues).</t>
-        </is>
-      </c>
-      <c r="C49" s="3" t="inlineStr">
-        <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D49" s="3" t="inlineStr">
-        <is>
-          <t>Yes, No</t>
-        </is>
-      </c>
-      <c r="E49" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F49" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G49" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-    </row>
-    <row r="50" ht="143" customHeight="1">
-      <c r="A50" s="3" t="inlineStr">
-        <is>
-          <t>If the response provides citations. Are the citations accurate/valid?</t>
-        </is>
-      </c>
-      <c r="B50" s="3" t="inlineStr">
-        <is>
-          <t>This means that the response can be found in the cited documents even if the response is not correct.
-Options are: 
-- accurate
-- partially accurate
-- inaccurate
-The latter one includes hallucinations.</t>
-        </is>
-      </c>
-      <c r="C50" s="3" t="inlineStr">
-        <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D50" s="3" t="inlineStr">
-        <is>
-          <t>accurate, partially accurate, inaccurate</t>
-        </is>
-      </c>
-      <c r="E50" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F50" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G50" s="3" t="inlineStr">
-        <is>
-          <t>partially accurate</t>
-        </is>
-      </c>
-    </row>
-    <row r="51" ht="89" customHeight="1">
-      <c r="A51" s="3" t="inlineStr">
-        <is>
-          <t>Please provide all the links to the citations</t>
-        </is>
-      </c>
-      <c r="B51" s="3" t="inlineStr">
-        <is>
-          <t>Enter the links from the files or locations used in the response.</t>
-        </is>
-      </c>
-      <c r="C51" s="3" t="inlineStr">
-        <is>
-          <t>Free text</t>
-        </is>
-      </c>
-      <c r="D51" s="3" t="inlineStr"/>
-      <c r="E51" s="3" t="inlineStr">
-        <is>
-          <t>Multiple</t>
-        </is>
-      </c>
-      <c r="F51" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G51" s="3" t="inlineStr">
-        <is>
-          <t>General_AcademicMajors_List_Vietnam_2024.pdf</t>
-        </is>
-      </c>
-    </row>
-    <row r="52" ht="89" customHeight="1">
-      <c r="A52" s="3" t="inlineStr">
-        <is>
-          <t>Overall what is the quality of the response?</t>
-        </is>
-      </c>
-      <c r="B52" s="3" t="inlineStr">
-        <is>
-          <t>Overall, what is the quality of the response? If you were an end user, would you use this response?</t>
-        </is>
-      </c>
-      <c r="C52" s="3" t="inlineStr">
-        <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D52" s="3" t="inlineStr">
-        <is>
-          <t>Good, Acceptable, Bad</t>
-        </is>
-      </c>
-      <c r="E52" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F52" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G52" s="3" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-    </row>
-    <row r="53" ht="107" customHeight="1">
-      <c r="A53" s="3" t="inlineStr">
-        <is>
-          <t>What aspects of the response make it good quality (if applicable)?</t>
-        </is>
-      </c>
-      <c r="B53" s="3" t="inlineStr">
-        <is>
-          <t>Please explain in what way the response is showing that it is of good quality</t>
-        </is>
-      </c>
-      <c r="C53" s="3" t="inlineStr">
-        <is>
-          <t>Free text</t>
-        </is>
-      </c>
-      <c r="D53" s="3" t="inlineStr"/>
-      <c r="E53" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F53" s="3" t="inlineStr">
-        <is>
-          <t>Optional</t>
-        </is>
-      </c>
-      <c r="G53" s="3" t="inlineStr"/>
-    </row>
-    <row r="54" ht="107" customHeight="1">
-      <c r="A54" s="3" t="inlineStr">
-        <is>
-          <t>What aspects of the response make it poor quality (if applicable)?</t>
-        </is>
-      </c>
-      <c r="B54" s="3" t="inlineStr">
-        <is>
-          <t>Please explain in what way the response is deficient or lacking</t>
-        </is>
-      </c>
-      <c r="C54" s="3" t="inlineStr">
-        <is>
-          <t>Free text</t>
-        </is>
-      </c>
-      <c r="D54" s="3" t="inlineStr"/>
-      <c r="E54" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F54" s="3" t="inlineStr">
-        <is>
-          <t>Optional</t>
-        </is>
-      </c>
-      <c r="G54" s="3" t="inlineStr">
-        <is>
-          <t>The MCS response gives information ungrounded in the knowldege corpus</t>
-        </is>
-      </c>
-    </row>
-    <row r="55" ht="107" customHeight="1">
-      <c r="A55" s="3" t="inlineStr">
-        <is>
-          <t>Any additional comments or reasoning for the rating? Optional</t>
-        </is>
-      </c>
-      <c r="B55" s="3" t="inlineStr"/>
-      <c r="C55" s="3" t="inlineStr">
-        <is>
-          <t>Free text</t>
-        </is>
-      </c>
-      <c r="D55" s="3" t="inlineStr"/>
-      <c r="E55" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F55" s="3" t="inlineStr">
-        <is>
-          <t>Optional</t>
-        </is>
-      </c>
-      <c r="G55" s="3" t="inlineStr"/>
-    </row>
-    <row r="56" ht="107" customHeight="1">
-      <c r="A56" s="3" t="inlineStr">
-        <is>
-          <t>Did the agent follow the given instructions or context?</t>
-        </is>
-      </c>
-      <c r="B56" s="3" t="inlineStr"/>
-      <c r="C56" s="3" t="inlineStr">
-        <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D56" s="3" t="inlineStr">
-        <is>
-          <t>completely followed, partially followed, did not follow</t>
-        </is>
-      </c>
-      <c r="E56" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F56" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G56" s="3" t="inlineStr">
-        <is>
-          <t>completely followed</t>
-        </is>
-      </c>
-    </row>
-    <row r="57" ht="143" customHeight="1">
-      <c r="A57" s="3" t="inlineStr">
-        <is>
-          <t>Logical flow, transitions, sentence structure.</t>
-        </is>
-      </c>
-      <c r="B57" s="3" t="inlineStr">
-        <is>
-          <t>How is the given layout and structure helping to understand the response?
-Could it have been organized and flowed in a way that made more sense?
-Rate between 1 (very bad) and 5 (very good)</t>
-        </is>
-      </c>
-      <c r="C57" s="3" t="inlineStr">
-        <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D57" s="3" t="inlineStr">
-        <is>
-          <t>1, 2, 3, 4, 5</t>
-        </is>
-      </c>
-      <c r="E57" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F57" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G57" s="3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-    </row>
-    <row r="58" ht="107" customHeight="1">
-      <c r="A58" s="3" t="inlineStr">
-        <is>
-          <t>Does it sound fluent and natural to a native speaker?</t>
-        </is>
-      </c>
-      <c r="B58" s="3" t="inlineStr">
-        <is>
-          <t>How is the quality of the grammar and natural use of English?
-Rate between 1 (very bad) and 5 (very good)</t>
-        </is>
-      </c>
-      <c r="C58" s="3" t="inlineStr">
-        <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D58" s="3" t="inlineStr">
-        <is>
-          <t>1, 2, 3, 4, 5</t>
-        </is>
-      </c>
-      <c r="E58" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F58" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G58" s="3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="59" ht="89" customHeight="1">
-      <c r="A59" s="3" t="inlineStr">
-        <is>
-          <t>Check if content is biased, harmful, or toxic.</t>
-        </is>
-      </c>
-      <c r="B59" s="3" t="inlineStr"/>
-      <c r="C59" s="3" t="inlineStr">
-        <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D59" s="3" t="inlineStr">
-        <is>
-          <t>Yes, No</t>
-        </is>
-      </c>
-      <c r="E59" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F59" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G59" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="60" ht="161" customHeight="1">
-      <c r="A60" s="3" t="inlineStr">
-        <is>
-          <t>What is the clarity of response?</t>
-        </is>
-      </c>
-      <c r="B60" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Is the response clear?
-Options are:
-Yes,No
-Yes: Response used simpler wording, explained terms or acronyms clearly and avoided technical jargon.
-No: Otherwise No
-It is directly tied to the "Clarity" dimension in the benchmarking rubric.</t>
-        </is>
-      </c>
-      <c r="C60" s="3" t="inlineStr">
-        <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D60" s="3" t="inlineStr">
-        <is>
-          <t>Yes, No</t>
-        </is>
-      </c>
-      <c r="E60" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F60" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G60" s="3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-    </row>
-    <row r="61" ht="107" customHeight="1">
-      <c r="A61" s="3" t="inlineStr">
-        <is>
-          <t>What is the tone and writing style of the agent response?</t>
-        </is>
-      </c>
-      <c r="B61" s="3" t="inlineStr">
-        <is>
-          <t>Options are:
-- Formal and conversational
-- Informal
-- Non-conversational</t>
-        </is>
-      </c>
-      <c r="C61" s="3" t="inlineStr">
-        <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D61" s="3" t="inlineStr">
-        <is>
-          <t>Formal and conversational,Informal,Non-conversational</t>
-        </is>
-      </c>
-      <c r="E61" s="3" t="inlineStr">
-        <is>
-          <t>Single</t>
-        </is>
-      </c>
-      <c r="F61" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G61" s="3" t="inlineStr">
-        <is>
-          <t>Formal and conversational</t>
-        </is>
-      </c>
-    </row>
-    <row r="62" ht="161" customHeight="1">
-      <c r="A62" s="3" t="inlineStr">
-        <is>
-          <t>Custom Rubric Used</t>
-        </is>
-      </c>
-      <c r="B62" s="3" t="inlineStr">
         <is>
           <t>The custom rubric contains one or multiple rubric criteria (questions related to the current query - can be different for each query)
 * Separate each rubric criterion by an in-cell line break (double click in the field -&gt; ALT+ENTER)</t>
         </is>
       </c>
-      <c r="C62" s="3" t="inlineStr">
+      <c r="C46" s="3" t="inlineStr">
         <is>
           <t>Free text</t>
         </is>
       </c>
-      <c r="D62" s="3" t="inlineStr"/>
-      <c r="E62" s="3" t="inlineStr">
+      <c r="D46" s="3" t="inlineStr"/>
+      <c r="E46" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F62" s="3" t="inlineStr"/>
-      <c r="G62" s="3" t="inlineStr">
+      <c r="F46" s="3" t="inlineStr"/>
+      <c r="G46" s="3" t="inlineStr">
         <is>
           <t>Includes clear and concise advice for effective CPR if the patient is pulseless or not breathing, such as high-quality compressions at 100-120 beats/min.
 Advises locating an AED if the patient is pulseless or not breathing.
@@ -3528,30 +2719,30 @@
         </is>
       </c>
     </row>
-    <row r="63" ht="71" customHeight="1">
-      <c r="A63" s="3" t="inlineStr">
+    <row r="47" ht="71" customHeight="1">
+      <c r="A47" s="3" t="inlineStr">
         <is>
           <t>Scores Per Rubric</t>
         </is>
       </c>
-      <c r="B63" s="3" t="inlineStr">
+      <c r="B47" s="3" t="inlineStr">
         <is>
           <t>This is a range between -10 and +10</t>
         </is>
       </c>
-      <c r="C63" s="3" t="inlineStr">
+      <c r="C47" s="3" t="inlineStr">
         <is>
           <t>Number</t>
         </is>
       </c>
-      <c r="D63" s="3" t="inlineStr"/>
-      <c r="E63" s="3" t="inlineStr">
+      <c r="D47" s="3" t="inlineStr"/>
+      <c r="E47" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F63" s="3" t="inlineStr"/>
-      <c r="G63" s="3" t="inlineStr">
+      <c r="F47" s="3" t="inlineStr"/>
+      <c r="G47" s="3" t="inlineStr">
         <is>
           <t>+8
 +8
@@ -3559,35 +2750,35 @@
         </is>
       </c>
     </row>
-    <row r="64" ht="125" customHeight="1">
-      <c r="A64" s="3" t="inlineStr">
+    <row r="48" ht="125" customHeight="1">
+      <c r="A48" s="3" t="inlineStr">
         <is>
           <t>Final Rubric Score</t>
         </is>
       </c>
-      <c r="B64" s="3" t="inlineStr">
+      <c r="B48" s="3" t="inlineStr">
         <is>
           <t>If the score given is greater than 0, the final rubric score if Yes
 If the score given is lower than or equal to 0, the final rubric score is No</t>
         </is>
       </c>
-      <c r="C64" s="3" t="inlineStr">
+      <c r="C48" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D64" s="3" t="inlineStr">
+      <c r="D48" s="3" t="inlineStr">
         <is>
           <t>Yes, No</t>
         </is>
       </c>
-      <c r="E64" s="3" t="inlineStr">
+      <c r="E48" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
         </is>
       </c>
-      <c r="F64" s="3" t="inlineStr"/>
-      <c r="G64" s="3" t="inlineStr">
+      <c r="F48" s="3" t="inlineStr"/>
+      <c r="G48" s="3" t="inlineStr">
         <is>
           <t>Yes
 Yes 
@@ -3595,81 +2786,125 @@
         </is>
       </c>
     </row>
-    <row r="65" ht="269" customHeight="1">
-      <c r="A65" s="3" t="inlineStr">
+    <row r="49" ht="71" customHeight="1">
+      <c r="A49" s="3" t="inlineStr">
         <is>
           <t>Pass/Fail</t>
         </is>
       </c>
-      <c r="B65" s="3" t="inlineStr">
-        <is>
-          <t>Fail if: 
-Does the agent response answer the question? --&gt; partially answers, does not answer
-What is the quality of the response? --&gt; bad
-Is the response comprehensive? --&gt; Somewhat comprehensive, not comprehensive
-Is the response correct? --&gt; Partially correct, incorrect
-If the response provides citations. Are the citations accurate? --&gt; partially accurate, inaccurate
-Did the agent follow the instructions? ---&gt; partially followed, did not follow</t>
-        </is>
-      </c>
-      <c r="C65" s="3" t="inlineStr">
+      <c r="B49" s="3" t="inlineStr"/>
+      <c r="C49" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
         </is>
       </c>
-      <c r="D65" s="3" t="inlineStr">
+      <c r="D49" s="3" t="inlineStr">
         <is>
           <t>Pass, Fail</t>
         </is>
       </c>
-      <c r="E65" s="3" t="inlineStr">
+      <c r="E49" s="3" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="F65" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G65" s="3" t="inlineStr">
+      <c r="F49" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G49" s="3" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
     </row>
-    <row r="66" ht="71" customHeight="1">
-      <c r="A66" s="3" t="inlineStr">
+    <row r="50" ht="71" customHeight="1">
+      <c r="A50" s="3" t="inlineStr">
         <is>
           <t>Justification for fail</t>
         </is>
       </c>
-      <c r="B66" s="3" t="inlineStr">
+      <c r="B50" s="3" t="inlineStr">
         <is>
           <t>Give a short description why you selected Fail.</t>
         </is>
       </c>
-      <c r="C66" s="3" t="inlineStr">
+      <c r="C50" s="3" t="inlineStr">
         <is>
           <t>Free text</t>
         </is>
       </c>
-      <c r="D66" s="3" t="inlineStr"/>
-      <c r="E66" s="3" t="inlineStr">
+      <c r="D50" s="3" t="inlineStr"/>
+      <c r="E50" s="3" t="inlineStr">
         <is>
           <t>Single</t>
         </is>
       </c>
-      <c r="F66" s="3" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
-      <c r="G66" s="3" t="inlineStr">
+      <c r="F50" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G50" s="3" t="inlineStr">
         <is>
           <t>MCS response gives info ungrounded in knowledge corpus (incorrect score that's needed to qualify for the IELTS requirement)</t>
         </is>
       </c>
+    </row>
+    <row r="51" ht="71" customHeight="1">
+      <c r="A51" s="3" t="inlineStr">
+        <is>
+          <t>Success score (1-5)</t>
+        </is>
+      </c>
+      <c r="B51" s="3" t="inlineStr"/>
+      <c r="C51" s="3" t="inlineStr">
+        <is>
+          <t>Number</t>
+        </is>
+      </c>
+      <c r="D51" s="3" t="inlineStr">
+        <is>
+          <t>1,2,3,4,5</t>
+        </is>
+      </c>
+      <c r="E51" s="3" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="F51" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G51" s="3" t="inlineStr"/>
+    </row>
+    <row r="52" ht="71" customHeight="1">
+      <c r="A52" s="3" t="inlineStr">
+        <is>
+          <t>Justification for Success score</t>
+        </is>
+      </c>
+      <c r="B52" s="3" t="inlineStr"/>
+      <c r="C52" s="3" t="inlineStr">
+        <is>
+          <t>Free text</t>
+        </is>
+      </c>
+      <c r="D52" s="3" t="inlineStr"/>
+      <c r="E52" s="3" t="inlineStr">
+        <is>
+          <t>Single</t>
+        </is>
+      </c>
+      <c r="F52" s="3" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="G52" s="3" t="inlineStr"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1" sheet="1" objects="0" insertRows="0" insertHyperlinks="0" autoFilter="0" scenarios="0" formatColumns="0" deleteColumns="0" insertColumns="0" pivotTables="0" deleteRows="0" formatCells="0" formatRows="0" sort="0"/>
@@ -3683,7 +2918,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK2"/>
+  <dimension ref="A1:AW2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -3704,15 +2939,15 @@
     <col width="21" customWidth="1" min="10" max="10"/>
     <col width="53" customWidth="1" min="11" max="11"/>
     <col width="40" customWidth="1" min="12" max="12"/>
-    <col width="40" customWidth="1" min="13" max="13"/>
-    <col width="59" customWidth="1" min="14" max="14"/>
-    <col width="30" customWidth="1" min="15" max="15"/>
-    <col width="29" customWidth="1" min="16" max="16"/>
-    <col width="16" customWidth="1" min="17" max="17"/>
-    <col width="86" customWidth="1" min="18" max="18"/>
+    <col width="59" customWidth="1" min="13" max="13"/>
+    <col width="29" customWidth="1" min="14" max="14"/>
+    <col width="28" customWidth="1" min="15" max="15"/>
+    <col width="16" customWidth="1" min="16" max="16"/>
+    <col width="86" customWidth="1" min="17" max="17"/>
+    <col width="15" customWidth="1" min="18" max="18"/>
     <col width="15" customWidth="1" min="19" max="19"/>
-    <col width="15" customWidth="1" min="20" max="20"/>
-    <col width="16" customWidth="1" min="21" max="21"/>
+    <col width="16" customWidth="1" min="20" max="20"/>
+    <col width="15" customWidth="1" min="21" max="21"/>
     <col width="15" customWidth="1" min="22" max="22"/>
     <col width="15" customWidth="1" min="23" max="23"/>
     <col width="15" customWidth="1" min="24" max="24"/>
@@ -3720,41 +2955,27 @@
     <col width="15" customWidth="1" min="26" max="26"/>
     <col width="15" customWidth="1" min="27" max="27"/>
     <col width="15" customWidth="1" min="28" max="28"/>
-    <col width="15" customWidth="1" min="29" max="29"/>
-    <col width="21" customWidth="1" min="30" max="30"/>
-    <col width="15" customWidth="1" min="31" max="31"/>
-    <col width="21" customWidth="1" min="32" max="32"/>
-    <col width="22" customWidth="1" min="33" max="33"/>
+    <col width="21" customWidth="1" min="29" max="29"/>
+    <col width="15" customWidth="1" min="30" max="30"/>
+    <col width="21" customWidth="1" min="31" max="31"/>
+    <col width="22" customWidth="1" min="32" max="32"/>
+    <col width="17" customWidth="1" min="33" max="33"/>
     <col width="17" customWidth="1" min="34" max="34"/>
     <col width="17" customWidth="1" min="35" max="35"/>
-    <col width="17" customWidth="1" min="36" max="36"/>
-    <col width="18" customWidth="1" min="37" max="37"/>
-    <col width="33" customWidth="1" min="38" max="38"/>
-    <col width="21" customWidth="1" min="39" max="39"/>
-    <col width="19" customWidth="1" min="40" max="40"/>
-    <col width="42" customWidth="1" min="41" max="41"/>
-    <col width="46" customWidth="1" min="42" max="42"/>
-    <col width="32" customWidth="1" min="43" max="43"/>
-    <col width="26" customWidth="1" min="44" max="44"/>
-    <col width="36" customWidth="1" min="45" max="45"/>
-    <col width="43" customWidth="1" min="46" max="46"/>
-    <col width="71" customWidth="1" min="47" max="47"/>
-    <col width="47" customWidth="1" min="48" max="48"/>
-    <col width="46" customWidth="1" min="49" max="49"/>
-    <col width="68" customWidth="1" min="50" max="50"/>
-    <col width="68" customWidth="1" min="51" max="51"/>
-    <col width="63" customWidth="1" min="52" max="52"/>
-    <col width="57" customWidth="1" min="53" max="53"/>
-    <col width="48" customWidth="1" min="54" max="54"/>
-    <col width="55" customWidth="1" min="55" max="55"/>
-    <col width="48" customWidth="1" min="56" max="56"/>
-    <col width="34" customWidth="1" min="57" max="57"/>
-    <col width="59" customWidth="1" min="58" max="58"/>
-    <col width="20" customWidth="1" min="59" max="59"/>
-    <col width="19" customWidth="1" min="60" max="60"/>
-    <col width="20" customWidth="1" min="61" max="61"/>
-    <col width="15" customWidth="1" min="62" max="62"/>
-    <col width="24" customWidth="1" min="63" max="63"/>
+    <col width="18" customWidth="1" min="36" max="36"/>
+    <col width="33" customWidth="1" min="37" max="37"/>
+    <col width="21" customWidth="1" min="38" max="38"/>
+    <col width="19" customWidth="1" min="39" max="39"/>
+    <col width="25" customWidth="1" min="40" max="40"/>
+    <col width="25" customWidth="1" min="41" max="41"/>
+    <col width="42" customWidth="1" min="42" max="42"/>
+    <col width="20" customWidth="1" min="43" max="43"/>
+    <col width="19" customWidth="1" min="44" max="44"/>
+    <col width="20" customWidth="1" min="45" max="45"/>
+    <col width="15" customWidth="1" min="46" max="46"/>
+    <col width="24" customWidth="1" min="47" max="47"/>
+    <col width="21" customWidth="1" min="48" max="48"/>
+    <col width="33" customWidth="1" min="49" max="49"/>
   </cols>
   <sheetData>
     <row r="1" ht="45" customHeight="1">
@@ -3815,262 +3036,192 @@
       </c>
       <c r="L1" s="5" t="inlineStr">
         <is>
-          <t>Number of files needed to answer query</t>
+          <t>Can be answered from knowledge corpus?</t>
         </is>
       </c>
       <c r="M1" s="5" t="inlineStr">
         <is>
-          <t>Can be answered from knowledge corpus?</t>
+          <t>Justification if cannot be answered from knowledge corpus</t>
         </is>
       </c>
       <c r="N1" s="5" t="inlineStr">
         <is>
-          <t>Justification if cannot be answered from knowledge corpus</t>
+          <t>Ground truth file reference</t>
         </is>
       </c>
       <c r="O1" s="5" t="inlineStr">
         <is>
-          <t>Ground truth file reference1</t>
+          <t>Knowledge corpus file type</t>
         </is>
       </c>
       <c r="P1" s="5" t="inlineStr">
         <is>
-          <t>Knowledge corpus file type2</t>
+          <t>File size type</t>
         </is>
       </c>
       <c r="Q1" s="5" t="inlineStr">
         <is>
-          <t>File size type</t>
+          <t>File size for PDFs, Power Point, Word doc, Text, SharePoint library docs, Worksheets</t>
         </is>
       </c>
       <c r="R1" s="5" t="inlineStr">
         <is>
-          <t>File size for PDFs, Power Point, Word doc, Text, SharePoint library docs, Worksheets</t>
+          <t>Textual body</t>
         </is>
       </c>
       <c r="S1" s="5" t="inlineStr">
         <is>
-          <t>Textual body</t>
+          <t>Simple Header</t>
         </is>
       </c>
       <c r="T1" s="5" t="inlineStr">
         <is>
-          <t>Simple Header</t>
+          <t>Complex Header</t>
         </is>
       </c>
       <c r="U1" s="5" t="inlineStr">
         <is>
-          <t>Complex Header</t>
+          <t>Footnotes</t>
         </is>
       </c>
       <c r="V1" s="5" t="inlineStr">
         <is>
-          <t>Footnotes</t>
+          <t>Simple Table</t>
         </is>
       </c>
       <c r="W1" s="5" t="inlineStr">
         <is>
-          <t>Simple Table</t>
+          <t>Complex Table</t>
         </is>
       </c>
       <c r="X1" s="5" t="inlineStr">
         <is>
-          <t>Complex Table</t>
+          <t>PDF images</t>
         </is>
       </c>
       <c r="Y1" s="5" t="inlineStr">
         <is>
-          <t>PDF images</t>
+          <t>Charts</t>
         </is>
       </c>
       <c r="Z1" s="5" t="inlineStr">
         <is>
-          <t>Charts</t>
+          <t>Simple list</t>
         </is>
       </c>
       <c r="AA1" s="5" t="inlineStr">
         <is>
-          <t>Simple list</t>
+          <t>Complex list</t>
         </is>
       </c>
       <c r="AB1" s="5" t="inlineStr">
         <is>
-          <t>Complex list</t>
+          <t>Metadata</t>
         </is>
       </c>
       <c r="AC1" s="5" t="inlineStr">
         <is>
-          <t>Metadata</t>
-        </is>
-      </c>
-      <c r="AD1" s="5" t="inlineStr">
-        <is>
           <t>Content Page Number</t>
         </is>
       </c>
+      <c r="AD1" s="6" t="inlineStr">
+        <is>
+          <t>User Query</t>
+        </is>
+      </c>
       <c r="AE1" s="6" t="inlineStr">
         <is>
-          <t>User Query</t>
+          <t>Clarity of question</t>
         </is>
       </c>
       <c r="AF1" s="6" t="inlineStr">
         <is>
-          <t>Clarity of question</t>
+          <t>User question intent</t>
         </is>
       </c>
       <c r="AG1" s="6" t="inlineStr">
         <is>
-          <t>User question intent</t>
+          <t>Question length</t>
         </is>
       </c>
       <c r="AH1" s="6" t="inlineStr">
         <is>
-          <t>Question length</t>
+          <t>Keyword queries</t>
         </is>
       </c>
       <c r="AI1" s="6" t="inlineStr">
         <is>
-          <t>Keyword queries</t>
+          <t>Spelling errors</t>
         </is>
       </c>
       <c r="AJ1" s="6" t="inlineStr">
         <is>
-          <t>Spelling errors</t>
+          <t>Doc term overlap</t>
         </is>
       </c>
       <c r="AK1" s="6" t="inlineStr">
         <is>
-          <t>Doc term overlap</t>
-        </is>
-      </c>
-      <c r="AL1" s="6" t="inlineStr">
-        <is>
           <t>Web search-engine-style queries</t>
         </is>
       </c>
+      <c r="AL1" s="7" t="inlineStr">
+        <is>
+          <t>MCS agent responses</t>
+        </is>
+      </c>
       <c r="AM1" s="7" t="inlineStr">
         <is>
-          <t>MCS agent responses</t>
+          <t>Expected response</t>
         </is>
       </c>
       <c r="AN1" s="7" t="inlineStr">
         <is>
-          <t>Expected response</t>
-        </is>
-      </c>
-      <c r="AO1" s="5" t="inlineStr">
+          <t>Expected tool selection</t>
+        </is>
+      </c>
+      <c r="AO1" s="7" t="inlineStr">
+        <is>
+          <t>Expeted tool parameters</t>
+        </is>
+      </c>
+      <c r="AP1" s="5" t="inlineStr">
         <is>
           <t>Ground truth snippets(Parsed) from files</t>
         </is>
       </c>
-      <c r="AP1" s="7" t="inlineStr">
-        <is>
-          <t>Does the agent response answer the question?</t>
-        </is>
-      </c>
-      <c r="AQ1" s="7" t="inlineStr">
-        <is>
-          <t>Is the response comprehensive?</t>
-        </is>
-      </c>
-      <c r="AR1" s="7" t="inlineStr">
-        <is>
-          <t>Is the response correct?</t>
-        </is>
-      </c>
-      <c r="AS1" s="7" t="inlineStr">
-        <is>
-          <t>Is the response's formatting good?</t>
-        </is>
-      </c>
-      <c r="AT1" s="7" t="inlineStr">
-        <is>
-          <t>Does the response provide citation links?</t>
-        </is>
-      </c>
-      <c r="AU1" s="7" t="inlineStr">
-        <is>
-          <t>If the response provides citations. Are the citations accurate/valid?</t>
-        </is>
-      </c>
-      <c r="AV1" s="7" t="inlineStr">
-        <is>
-          <t>Please provide all the links to the citations</t>
-        </is>
-      </c>
-      <c r="AW1" s="7" t="inlineStr">
-        <is>
-          <t>Overall what is the quality of the response?</t>
-        </is>
-      </c>
-      <c r="AX1" s="7" t="inlineStr">
-        <is>
-          <t>What aspects of the response make it good quality (if applicable)?</t>
-        </is>
-      </c>
-      <c r="AY1" s="7" t="inlineStr">
-        <is>
-          <t>What aspects of the response make it poor quality (if applicable)?</t>
-        </is>
-      </c>
-      <c r="AZ1" s="7" t="inlineStr">
-        <is>
-          <t>Any additional comments or reasoning for the rating? Optional</t>
-        </is>
-      </c>
-      <c r="BA1" s="7" t="inlineStr">
-        <is>
-          <t>Did the agent follow the given instructions or context?</t>
-        </is>
-      </c>
-      <c r="BB1" s="7" t="inlineStr">
-        <is>
-          <t>Logical flow, transitions, sentence structure.</t>
-        </is>
-      </c>
-      <c r="BC1" s="7" t="inlineStr">
-        <is>
-          <t>Does it sound fluent and natural to a native speaker?</t>
-        </is>
-      </c>
-      <c r="BD1" s="7" t="inlineStr">
-        <is>
-          <t>Check if content is biased, harmful, or toxic.</t>
-        </is>
-      </c>
-      <c r="BE1" s="7" t="inlineStr">
-        <is>
-          <t>What is the clarity of response?</t>
-        </is>
-      </c>
-      <c r="BF1" s="7" t="inlineStr">
-        <is>
-          <t>What is the tone and writing style of the agent response?</t>
-        </is>
-      </c>
-      <c r="BG1" s="8" t="inlineStr">
+      <c r="AQ1" s="8" t="inlineStr">
         <is>
           <t>Custom Rubric Used</t>
         </is>
       </c>
-      <c r="BH1" s="8" t="inlineStr">
+      <c r="AR1" s="8" t="inlineStr">
         <is>
           <t>Scores Per Rubric</t>
         </is>
       </c>
-      <c r="BI1" s="8" t="inlineStr">
+      <c r="AS1" s="8" t="inlineStr">
         <is>
           <t>Final Rubric Score</t>
         </is>
       </c>
-      <c r="BJ1" s="9" t="inlineStr">
+      <c r="AT1" s="9" t="inlineStr">
         <is>
           <t>Pass/Fail</t>
         </is>
       </c>
-      <c r="BK1" s="9" t="inlineStr">
+      <c r="AU1" s="9" t="inlineStr">
         <is>
           <t>Justification for fail</t>
+        </is>
+      </c>
+      <c r="AV1" s="9" t="inlineStr">
+        <is>
+          <t>Success score (1-5)</t>
+        </is>
+      </c>
+      <c r="AW1" s="9" t="inlineStr">
+        <is>
+          <t>Justification for Success score</t>
         </is>
       </c>
     </row>
@@ -4124,41 +3275,27 @@
       <c r="AU2" s="10" t="n"/>
       <c r="AV2" s="10" t="n"/>
       <c r="AW2" s="10" t="n"/>
-      <c r="AX2" s="10" t="n"/>
-      <c r="AY2" s="10" t="n"/>
-      <c r="AZ2" s="10" t="n"/>
-      <c r="BA2" s="10" t="n"/>
-      <c r="BB2" s="10" t="n"/>
-      <c r="BC2" s="10" t="n"/>
-      <c r="BD2" s="10" t="n"/>
-      <c r="BE2" s="10" t="n"/>
-      <c r="BF2" s="10" t="n"/>
-      <c r="BG2" s="10" t="n"/>
-      <c r="BH2" s="10" t="n"/>
-      <c r="BI2" s="10" t="n"/>
-      <c r="BJ2" s="10" t="n"/>
-      <c r="BK2" s="10" t="n"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BK1"/>
-  <dataValidations count="40">
+  <autoFilter ref="A1:AW1"/>
+  <dataValidations count="27">
     <dataValidation sqref="A2:A1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation sqref="L2:L1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
+    <dataValidation sqref="L2:L1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation sqref="P2:P1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Small,Medium,Large"</formula1>
+    </dataValidation>
+    <dataValidation sqref="Q2:Q1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation sqref="M2:M1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="R2:R1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation sqref="Q2:Q1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Small,Medium,Large"</formula1>
-    </dataValidation>
-    <dataValidation sqref="R2:R1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
-      <formula1>0</formula1>
     </dataValidation>
     <dataValidation sqref="S2:S1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"Yes,No"</formula1>
@@ -4190,14 +3327,14 @@
     <dataValidation sqref="AB2:AB1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="AC2:AC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation sqref="AD2:AD1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
+    <dataValidation sqref="AC2:AC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation sqref="AF2:AF1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="AE2:AE1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"Low,Medium,High"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AH2:AH1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation sqref="AI2:AI1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"Yes,No"</formula1>
@@ -4208,59 +3345,20 @@
     <dataValidation sqref="AK2:AK1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="AL2:AL1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+    <dataValidation sqref="AP2:AP1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation sqref="AR2:AR1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation sqref="AS2:AS1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation sqref="AO2:AO1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
+    <dataValidation sqref="AT2:AT1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>"Pass,Fail"</formula1>
+    </dataValidation>
+    <dataValidation sqref="AV2:AV1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
       <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation sqref="AP2:AP1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation sqref="AQ2:AQ1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Fully comprehensive,Somewhat comprehensive,Not applicable"</formula1>
-    </dataValidation>
-    <dataValidation sqref="AR2:AR1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Fully correct,Partially correct,Incorrect."</formula1>
-    </dataValidation>
-    <dataValidation sqref="AS2:AS1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation sqref="AT2:AT1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation sqref="AU2:AU1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"accurate,partially accurate,inaccurate"</formula1>
-    </dataValidation>
-    <dataValidation sqref="AW2:AW1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Good,Acceptable,Bad"</formula1>
-    </dataValidation>
-    <dataValidation sqref="BA2:BA1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"completely followed,partially followed,did not follow"</formula1>
-    </dataValidation>
-    <dataValidation sqref="BB2:BB1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"1,2,3,4,5"</formula1>
-    </dataValidation>
-    <dataValidation sqref="BC2:BC1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"1,2,3,4,5"</formula1>
-    </dataValidation>
-    <dataValidation sqref="BD2:BD1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation sqref="BE2:BE1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation sqref="BF2:BF1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Formal and conversational,Informal,Non-conversational"</formula1>
-    </dataValidation>
-    <dataValidation sqref="BH2:BH1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
-      <formula1>0</formula1>
-    </dataValidation>
-    <dataValidation sqref="BI2:BI1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation sqref="BJ2:BJ1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated to discussion status 20251009
</commit_message>
<xml_diff>
--- a/create_agent_directory/resources/enhanced_template.xlsx
+++ b/create_agent_directory/resources/enhanced_template.xlsx
@@ -662,8 +662,8 @@
     </comment>
     <comment ref="AP1" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">Expeted tool parameters
-The corresponding list of tool parameters for the expected tools
+        <t xml:space="preserve">Expected tool parameters and values
+The corresponding list of tool parameters for the expected tools along with expected values
 </t>
       </text>
     </comment>
@@ -2672,20 +2672,25 @@
       </c>
       <c r="F44" s="3" t="inlineStr">
         <is>
-          <t>Optional</t>
-        </is>
-      </c>
-      <c r="G44" s="3" t="inlineStr"/>
-    </row>
-    <row r="45" ht="71" customHeight="1">
+          <t>Required_for_orchestration</t>
+        </is>
+      </c>
+      <c r="G44" s="3" t="inlineStr">
+        <is>
+          <t>Query: Pay $1000 to my credit card and $2000 to my mortgage
+Expected tool election: ['Get_Account_Number', 'Get_Account_Number', 'Make_Payment', 'Make_Payment']</t>
+        </is>
+      </c>
+    </row>
+    <row r="45" ht="107" customHeight="1">
       <c r="A45" s="3" t="inlineStr">
         <is>
-          <t>Expeted tool parameters</t>
+          <t>Expected tool parameters and values</t>
         </is>
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>The corresponding list of tool parameters for the expected tools</t>
+          <t>The corresponding list of tool parameters for the expected tools along with expected values</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
@@ -2701,10 +2706,15 @@
       </c>
       <c r="F45" s="3" t="inlineStr">
         <is>
-          <t>Optional</t>
-        </is>
-      </c>
-      <c r="G45" s="3" t="inlineStr"/>
+          <t>Required_for_orchestration</t>
+        </is>
+      </c>
+      <c r="G45" s="3" t="inlineStr">
+        <is>
+          <t>Query: Query: Pay $1000 to my credit card and $2000 to my mortgage
+Expected parameter names and values: [{'user_id': 'felix', 'account_type': 'credit_card'}, {'user_id': 'felix', 'account_type': 'mortgage'}, {'account_number': '****1234', 'amount': 1000}, {'account_number': '****5678', 'amount': 2000}]</t>
+        </is>
+      </c>
     </row>
     <row r="46" ht="251" customHeight="1">
       <c r="A46" s="3" t="inlineStr">
@@ -3049,7 +3059,7 @@
     <col width="21" customWidth="1" min="39" max="39"/>
     <col width="19" customWidth="1" min="40" max="40"/>
     <col width="25" customWidth="1" min="41" max="41"/>
-    <col width="25" customWidth="1" min="42" max="42"/>
+    <col width="37" customWidth="1" min="42" max="42"/>
     <col width="42" customWidth="1" min="43" max="43"/>
     <col width="20" customWidth="1" min="44" max="44"/>
     <col width="19" customWidth="1" min="45" max="45"/>
@@ -3268,7 +3278,7 @@
       </c>
       <c r="AP1" s="7" t="inlineStr">
         <is>
-          <t>Expeted tool parameters</t>
+          <t>Expected tool parameters and values</t>
         </is>
       </c>
       <c r="AQ1" s="5" t="inlineStr">

</xml_diff>